<commit_message>
Ground Work for Matched Partners Strat
</commit_message>
<xml_diff>
--- a/Reference.xlsx
+++ b/Reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sudoku_Bitmask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5889DB45-57EC-4F3B-B9E4-A9895F6E5F8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCAC96C-7AA8-48B4-B431-2B4FB37BC761}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9195" windowHeight="6720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="6720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>X</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>0,0,8,3,0,0,9,0</t>
+  </si>
+  <si>
+    <t>1,4,7,28,31,34,55,58,61</t>
   </si>
 </sst>
 </file>
@@ -1372,26 +1375,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58:D60"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="V59" sqref="V59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="10" width="3" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="3" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.5546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.5546875" style="25" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="0" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="0" style="3" hidden="1" customWidth="1"/>
     <col min="19" max="20" width="0" hidden="1" customWidth="1"/>
-    <col min="29" max="37" width="2.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="29" max="37" width="2.88671875" style="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="L1" s="5" t="s">
         <v>3</v>
       </c>
@@ -1432,7 +1435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="22">
         <v>1</v>
       </c>
@@ -1502,7 +1505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
         <v>1</v>
       </c>
@@ -1575,7 +1578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
         <v>2</v>
       </c>
@@ -1648,7 +1651,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>3</v>
       </c>
@@ -1721,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
         <v>4</v>
       </c>
@@ -1794,7 +1797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
         <v>5</v>
       </c>
@@ -1867,7 +1870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>6</v>
       </c>
@@ -1940,7 +1943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>7</v>
       </c>
@@ -2013,7 +2016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>8</v>
       </c>
@@ -2086,7 +2089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="22">
         <v>9</v>
       </c>
@@ -2159,7 +2162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="L12" s="5">
         <v>11</v>
       </c>
@@ -2195,7 +2198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B13" s="6">
         <v>0</v>
       </c>
@@ -2258,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B14" s="9">
         <v>0</v>
       </c>
@@ -2321,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B15" s="17">
         <v>8</v>
       </c>
@@ -2384,7 +2387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B16" s="9">
         <v>0</v>
       </c>
@@ -2447,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B17" s="9">
         <v>3</v>
       </c>
@@ -2510,7 +2513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B18" s="17">
         <v>0</v>
       </c>
@@ -2573,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B19" s="9">
         <v>0</v>
       </c>
@@ -2636,7 +2639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B20" s="9">
         <v>9</v>
       </c>
@@ -2699,7 +2702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="12">
         <v>0</v>
       </c>
@@ -2762,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="L22" s="5">
         <v>21</v>
       </c>
@@ -2798,7 +2801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="L23" s="5">
         <v>22</v>
       </c>
@@ -2834,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="22">
         <v>1</v>
       </c>
@@ -2897,7 +2900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" s="22">
         <v>1</v>
       </c>
@@ -2963,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" s="22">
         <v>2</v>
       </c>
@@ -3029,7 +3032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="22">
         <v>3</v>
       </c>
@@ -3095,7 +3098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" s="22">
         <v>4</v>
       </c>
@@ -3161,7 +3164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" s="22">
         <v>5</v>
       </c>
@@ -3231,7 +3234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="22">
         <v>6</v>
       </c>
@@ -3297,7 +3300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" s="22">
         <v>7</v>
       </c>
@@ -3363,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" s="22">
         <v>8</v>
       </c>
@@ -3429,7 +3432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="22">
         <v>9</v>
       </c>
@@ -3495,7 +3498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="L34" s="5">
         <v>33</v>
       </c>
@@ -3531,7 +3534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" s="22">
         <v>1</v>
       </c>
@@ -3597,7 +3600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" s="22">
         <v>2</v>
       </c>
@@ -3663,7 +3666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" s="22">
         <v>3</v>
       </c>
@@ -3729,7 +3732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" s="22">
         <v>4</v>
       </c>
@@ -3798,7 +3801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" s="22">
         <v>5</v>
       </c>
@@ -3864,7 +3867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="22">
         <v>6</v>
       </c>
@@ -3930,7 +3933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="22">
         <v>7</v>
       </c>
@@ -3996,7 +3999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="22">
         <v>8</v>
       </c>
@@ -4062,7 +4065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="22">
         <v>9</v>
       </c>
@@ -4128,7 +4131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="L44" s="5">
         <v>43</v>
       </c>
@@ -4164,7 +4167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="L45" s="5">
         <v>44</v>
       </c>
@@ -4200,7 +4203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="L46" s="5">
         <v>45</v>
       </c>
@@ -4236,7 +4239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="L47" s="5">
         <v>46</v>
       </c>
@@ -4272,7 +4275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="L48" s="5">
         <v>47</v>
       </c>
@@ -4308,7 +4311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
       <c r="L49" s="5">
         <v>48</v>
       </c>
@@ -4344,7 +4347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
       <c r="L50" s="5">
         <v>49</v>
       </c>
@@ -4380,7 +4383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
       <c r="L51" s="5">
         <v>50</v>
       </c>
@@ -4416,7 +4419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
       <c r="L52" s="5">
         <v>51</v>
       </c>
@@ -4452,7 +4455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
       <c r="L53" s="5">
         <v>52</v>
       </c>
@@ -4488,7 +4491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
       <c r="L54" s="5">
         <v>53</v>
       </c>
@@ -4524,7 +4527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
       <c r="L55" s="5">
         <v>54</v>
       </c>
@@ -4560,7 +4563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
       <c r="L56" s="5">
         <v>55</v>
       </c>
@@ -4596,7 +4599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B57" s="22">
         <v>1</v>
       </c>
@@ -4659,7 +4662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A58" s="22">
         <v>1</v>
       </c>
@@ -4724,8 +4727,11 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A59" s="22">
         <v>2</v>
       </c>
@@ -4791,7 +4797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A60" s="22">
         <v>3</v>
       </c>
@@ -4857,7 +4863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A61" s="22">
         <v>4</v>
       </c>
@@ -4923,7 +4929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A62" s="22">
         <v>5</v>
       </c>
@@ -4989,7 +4995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A63" s="22">
         <v>6</v>
       </c>
@@ -5055,7 +5061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A64" s="22">
         <v>7</v>
       </c>
@@ -5121,7 +5127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" s="22">
         <v>8</v>
       </c>
@@ -5187,7 +5193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="22">
         <v>9</v>
       </c>
@@ -5253,7 +5259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L67" s="5">
         <v>66</v>
       </c>
@@ -5289,7 +5295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L68" s="5">
         <v>67</v>
       </c>
@@ -5325,7 +5331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L69" s="5">
         <v>68</v>
       </c>
@@ -5361,7 +5367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L70" s="5">
         <v>69</v>
       </c>
@@ -5397,7 +5403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L71" s="5">
         <v>70</v>
       </c>
@@ -5433,7 +5439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L72" s="5">
         <v>71</v>
       </c>
@@ -5469,7 +5475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L73" s="5">
         <v>72</v>
       </c>
@@ -5505,7 +5511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L74" s="5">
         <v>73</v>
       </c>
@@ -5541,7 +5547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L75" s="5">
         <v>74</v>
       </c>
@@ -5577,7 +5583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L76" s="5">
         <v>75</v>
       </c>
@@ -5613,7 +5619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L77" s="5">
         <v>76</v>
       </c>
@@ -5649,7 +5655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L78" s="5">
         <v>77</v>
       </c>
@@ -5685,7 +5691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L79" s="5">
         <v>78</v>
       </c>
@@ -5721,7 +5727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L80" s="5">
         <v>79</v>
       </c>
@@ -5757,7 +5763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="81" spans="12:20" x14ac:dyDescent="0.3">
       <c r="L81" s="5">
         <v>80</v>
       </c>
@@ -5793,7 +5799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="82" spans="12:20" x14ac:dyDescent="0.3">
       <c r="L82" s="5">
         <v>81</v>
       </c>

</xml_diff>